<commit_message>
UPDATE BOM & PCB file
</commit_message>
<xml_diff>
--- a/hardware/LamdaShifter_2_0_BOM.xlsx
+++ b/hardware/LamdaShifter_2_0_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\PlatformIO\Projects\Lambda Shifter OTA\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C9B9E4-40EA-4C4E-86DB-8A48BF532F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEAD912-D02A-417E-80D5-3BE4761793EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,14 +185,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>REG1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q1,Q2</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>D1,D2,D3</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -273,6 +265,14 @@
       </rPr>
       <t>Ω</t>
     </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q2,Q3</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -795,7 +795,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -880,7 +880,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -905,19 +905,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="11" t="s">
@@ -930,19 +930,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="11" t="s">
@@ -955,19 +955,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3">
         <v>2</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>19</v>
@@ -982,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3">
         <v>3</v>
@@ -1007,7 +1007,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
@@ -1015,7 +1015,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G9" s="10">
         <v>3216</v>
@@ -1030,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -1038,7 +1038,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G10" s="10">
         <v>3216</v>
@@ -1053,7 +1053,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -1061,7 +1061,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" s="10">
         <v>3216</v>

</xml_diff>